<commit_message>
Update Trebac Playback Data_November 2022.xlsx
</commit_message>
<xml_diff>
--- a/Trebac Playback Data_November 2022.xlsx
+++ b/Trebac Playback Data_November 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlytrebac/Documents/GitHub/WBNU-playback/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A12F092-41CE-334B-9D09-C55EB4A9D653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8D7C87-68A8-1145-83A1-72F8DFD4E573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1620" windowWidth="28800" windowHeight="16560" xr2:uid="{4C99C56D-1347-C14A-A596-296C23F96F99}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{4C99C56D-1347-C14A-A596-296C23F96F99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295DAB66-7475-AA48-91F2-E743C24A9A27}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>